<commit_message>
Small documentation improvements, 1 potential bug fix
Improved documentation of function inputs and outputs
Re-named model function so it matches model name
Added logic to test whether snow depth is being calculated before
appending it to results file.
</commit_message>
<xml_diff>
--- a/Example_Data/Parameters_v0-1A_Tarland.xlsx
+++ b/Example_Data/Parameters_v0-1A_Tarland.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="696" windowWidth="18192" windowHeight="11160"/>
+    <workbookView xWindow="480" yWindow="696" windowWidth="18192" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="8" r:id="rId1"/>
@@ -753,27 +753,12 @@
     <t>Q, SS, PP, TDP, TP</t>
   </si>
   <si>
-    <t>2004-01-01</t>
-  </si>
-  <si>
-    <t>2005-12-31</t>
-  </si>
-  <si>
     <t>point</t>
   </si>
   <si>
     <t>Keep constant unless strong reasons to do otherwise</t>
   </si>
   <si>
-    <t>C:\Data\GitHub\SimplyP\ModelInputs\Tarland_MetData_1981-2010.csv</t>
-  </si>
-  <si>
-    <t>C:\Data\GitHub\SimplyP\ModelInputs\Observations\Tarland\WholePeriod\Coull_DailyMeanQ.xlsx</t>
-  </si>
-  <si>
-    <t>C:\Data\GitHub\SimplyP\ModelInputs\Observations\Tarland\WholePeriod\Coull_ChemObs.xlsx</t>
-  </si>
-  <si>
     <t>C:\Data\GitHub\Output</t>
   </si>
   <si>
@@ -787,6 +772,21 @@
   </si>
   <si>
     <t>Format for value cell</t>
+  </si>
+  <si>
+    <t>2004-10-01</t>
+  </si>
+  <si>
+    <t>2005-09-30</t>
+  </si>
+  <si>
+    <t>C:\Data\GitHub\SimplyP\Example_Data\Tarland_MetData_1981-2010.csv</t>
+  </si>
+  <si>
+    <t>C:\Data\GitHub\SimplyP\Example_Data\Observations\Tarland\WholePeriod\Coull_ChemObs.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Data\GitHub\SimplyP\Example_Data\Observations\Tarland\WholePeriod\Coull_DailyMeanQ.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1965,7 +1965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
@@ -1980,15 +1980,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.6640625" style="38" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52.88671875" style="38" customWidth="1"/>
-    <col min="3" max="3" width="53.44140625" style="38" customWidth="1"/>
+    <col min="3" max="3" width="73.88671875" style="38" customWidth="1"/>
     <col min="4" max="4" width="53.5546875" style="38" customWidth="1"/>
     <col min="5" max="16384" width="9.109375" style="38"/>
   </cols>
@@ -2004,7 +2004,7 @@
         <v>24</v>
       </c>
       <c r="D1" s="41" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2015,7 +2015,7 @@
         <v>114</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="D2" s="36" t="s">
         <v>150</v>
@@ -2029,7 +2029,7 @@
         <v>116</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>237</v>
+        <v>243</v>
       </c>
       <c r="D3" s="36" t="s">
         <v>150</v>
@@ -2043,7 +2043,7 @@
         <v>118</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="D4" s="36" t="s">
         <v>150</v>
@@ -2057,7 +2057,7 @@
         <v>153</v>
       </c>
       <c r="C5" s="38" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D5" s="36" t="s">
         <v>150</v>
@@ -2071,7 +2071,7 @@
         <v>226</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D6" s="36" t="s">
         <v>227</v>
@@ -2099,7 +2099,7 @@
         <v>123</v>
       </c>
       <c r="C8" s="39" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="D8" s="36" t="s">
         <v>149</v>
@@ -2113,7 +2113,7 @@
         <v>124</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="D9" s="36" t="s">
         <v>149</v>
@@ -2295,13 +2295,13 @@
         <v>187</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D22" s="49" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="44" t="s">
         <v>178</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
         <v>181</v>
       </c>
@@ -2402,7 +2402,7 @@
       <c r="G2" s="114"/>
       <c r="H2" s="115"/>
       <c r="I2" s="116" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="124" customFormat="1" x14ac:dyDescent="0.25">
@@ -2427,7 +2427,7 @@
       <c r="G3" s="121"/>
       <c r="H3" s="122"/>
       <c r="I3" s="123" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="124" customFormat="1" x14ac:dyDescent="0.25">
@@ -2506,7 +2506,7 @@
       </c>
       <c r="H6" s="141"/>
       <c r="I6" s="142" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="108" customFormat="1" x14ac:dyDescent="0.25">
@@ -2533,7 +2533,7 @@
       </c>
       <c r="H7" s="145"/>
       <c r="I7" s="146" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -3036,7 +3036,7 @@
         <v>0.43</v>
       </c>
       <c r="F11" s="154" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="71" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -3513,7 +3513,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>209</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>210</v>
       </c>
@@ -3537,7 +3537,7 @@
         <v>1650</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>211</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>2650</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>147</v>
       </c>
@@ -3557,7 +3557,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
         <v>142</v>
       </c>
@@ -3565,7 +3565,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
         <v>143</v>
       </c>
@@ -3573,7 +3573,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
         <v>144</v>
       </c>

</xml_diff>

<commit_message>
Upload data associated with WRR article submission
Upload SimplyP and INCA-P data files associated with WRR article
submission, for reproduction of results.
</commit_message>
<xml_diff>
--- a/Example_Data/Parameters_v0-1A_Tarland.xlsx
+++ b/Example_Data/Parameters_v0-1A_Tarland.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="696" windowWidth="18192" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="690" windowWidth="18195" windowHeight="11160" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="8" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="233">
   <si>
     <t>Param</t>
   </si>
@@ -378,15 +378,6 @@
     <t>File path to chemistry observations</t>
   </si>
   <si>
-    <t>C:\Users\lj40184\Documents\GitHub\enviro_mod_notes\notebooks\ModelInputs\Tar_AvMetData_1981-2010.csv</t>
-  </si>
-  <si>
-    <t>C:\Users\lj40184\Documents\GitHub\enviro_mod_notes\notebooks\ModelInputs\obs_csvs\Coull_9amDailyMeanQ_oldRating.xlsx</t>
-  </si>
-  <si>
-    <t>C:\Users\lj40184\Documents\GitHub\enviro_mod_notes\notebooks\ModelInputs\obs_csvs\WholePeriod\TarChem_R4_SS-P.xlsx</t>
-  </si>
-  <si>
     <t>run_mode</t>
   </si>
   <si>
@@ -447,27 +438,12 @@
     <t>This sheet provides some simple aides to parameterising the model. It is not read in to the model</t>
   </si>
   <si>
-    <t>M:\Working\NewModel\ModelInputs\Tar_AvMetData_1981-2010.csv</t>
-  </si>
-  <si>
-    <t>M:\Working\NewModel\ModelInputs\obs_csvs\Coull_9amDailyMeanQ_oldRating.xlsx</t>
-  </si>
-  <si>
-    <t>M:\Working\NewModel\ModelInputs\obs_csvs\WholePeriod\TarChem_R4_SS-P.xlsx</t>
-  </si>
-  <si>
     <t>Only required if Dynamic_erodibility is set to 'y' in Setup parameters.</t>
   </si>
   <si>
     <t>Only required if Dynamic_erodibility is set to 'y' in Setup parameters. e.g. 1st of March. Conversion from Calendar day to Julian day, see e.g. http://landweb.nascom.nasa.gov/browse/calendar.html</t>
   </si>
   <si>
-    <t>File paths for work desktop:</t>
-  </si>
-  <si>
-    <t>File paths for work laptop:</t>
-  </si>
-  <si>
     <t>Text; format 'yyyy-mm-dd'</t>
   </si>
   <si>
@@ -655,9 +631,6 @@
   </si>
   <si>
     <t>Quartzite (rock)</t>
-  </si>
-  <si>
-    <t>Bulk densities (kg/m3)</t>
   </si>
   <si>
     <r>
@@ -741,15 +714,6 @@
     <t>Text: cal, val or scenario (case sensitive)</t>
   </si>
   <si>
-    <t>M:\Working\NewModel\ModelInputs\obs_csvs\Val\TarChem_R4_SS-P_val.xlsx</t>
-  </si>
-  <si>
-    <t>M:\Working\NewModel\ModelInputs\obs_csvs\Val\Coull_9amDailyMeanQ_oldRating_Val.xlsx</t>
-  </si>
-  <si>
-    <t>Val:</t>
-  </si>
-  <si>
     <t>Q, SS, PP, TDP, TP</t>
   </si>
   <si>
@@ -774,12 +738,6 @@
     <t>Format for value cell</t>
   </si>
   <si>
-    <t>2004-10-01</t>
-  </si>
-  <si>
-    <t>2005-09-30</t>
-  </si>
-  <si>
     <t>C:\Data\GitHub\SimplyP\Example_Data\Tarland_MetData_1981-2010.csv</t>
   </si>
   <si>
@@ -787,6 +745,15 @@
   </si>
   <si>
     <t>C:\Data\GitHub\SimplyP\Example_Data\Observations\Tarland\WholePeriod\Coull_DailyMeanQ.xlsx</t>
+  </si>
+  <si>
+    <t>2004-01-01</t>
+  </si>
+  <si>
+    <t>2005-04-30</t>
+  </si>
+  <si>
+    <t>Bulk density(kg/m3)</t>
   </si>
 </sst>
 </file>
@@ -1091,7 +1058,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1127,16 +1094,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1195,12 +1158,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1322,9 +1279,6 @@
     <xf numFmtId="11" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1343,61 +1297,16 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="11" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1423,6 +1332,198 @@
     </xf>
     <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="11" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1969,7 +2070,7 @@
       <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1980,353 +2081,353 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" style="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.88671875" style="38" customWidth="1"/>
-    <col min="3" max="3" width="73.88671875" style="38" customWidth="1"/>
-    <col min="4" max="4" width="53.5546875" style="38" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="38"/>
+    <col min="1" max="1" width="26.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.85546875" style="36" customWidth="1"/>
+    <col min="3" max="3" width="73.85546875" style="36" customWidth="1"/>
+    <col min="4" max="4" width="53.5703125" style="36" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="43" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="41" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="D1" s="39" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="C2" s="38" t="s">
-        <v>241</v>
-      </c>
-      <c r="D2" s="36" t="s">
+      <c r="C2" s="36" t="s">
+        <v>227</v>
+      </c>
+      <c r="D2" s="34" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="43" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="D4" s="34" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="42" t="s">
+        <v>144</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>222</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>217</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>230</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>231</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" s="36">
+        <v>1</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" s="46" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="42" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12" s="46" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="44" t="s">
+        <v>177</v>
+      </c>
+      <c r="B13" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" s="46" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="44" t="s">
+        <v>175</v>
+      </c>
+      <c r="B14" s="45" t="s">
+        <v>176</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D14" s="46" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="B15" s="45" t="s">
+        <v>164</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15" s="46" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="35" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="44" t="s">
+        <v>146</v>
+      </c>
+      <c r="B16" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D16" s="46" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="42" t="s">
+        <v>147</v>
+      </c>
+      <c r="B17" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="D17" s="46" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>157</v>
+      </c>
+      <c r="D18" s="47" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="42" t="s">
+        <v>159</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="C19" s="36">
+        <v>300</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="42" t="s">
+        <v>165</v>
+      </c>
+      <c r="B20" s="34" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3" s="45" t="s">
-        <v>116</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>243</v>
-      </c>
-      <c r="D3" s="36" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
-        <v>117</v>
-      </c>
-      <c r="B4" s="45" t="s">
-        <v>118</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>242</v>
-      </c>
-      <c r="D4" s="36" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+      <c r="C20" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="D20" s="47" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="42" t="s">
         <v>152</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B21" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="C5" s="38" t="s">
-        <v>234</v>
-      </c>
-      <c r="D5" s="36" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="s">
-        <v>122</v>
-      </c>
-      <c r="B6" s="45" t="s">
-        <v>226</v>
-      </c>
-      <c r="C6" s="38" t="s">
-        <v>235</v>
-      </c>
-      <c r="D6" s="36" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
-        <v>135</v>
-      </c>
-      <c r="B7" s="45" t="s">
-        <v>136</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>131</v>
-      </c>
-      <c r="D7" s="36" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
-        <v>125</v>
-      </c>
-      <c r="B8" s="45" t="s">
-        <v>123</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>239</v>
-      </c>
-      <c r="D8" s="36" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="44" t="s">
-        <v>126</v>
-      </c>
-      <c r="B9" s="45" t="s">
-        <v>124</v>
-      </c>
-      <c r="C9" s="39" t="s">
-        <v>240</v>
-      </c>
-      <c r="D9" s="36" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="44" t="s">
-        <v>127</v>
-      </c>
-      <c r="B10" s="45" t="s">
-        <v>128</v>
-      </c>
-      <c r="C10" s="38">
-        <v>1</v>
-      </c>
-      <c r="D10" s="36" t="s">
+      <c r="C21" s="36" t="s">
+        <v>219</v>
+      </c>
+      <c r="D21" s="47" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="42" t="s">
+        <v>166</v>
+      </c>
+      <c r="B22" s="43" t="s">
+        <v>179</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>220</v>
+      </c>
+      <c r="D22" s="47" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A23" s="42" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="B11" s="45" t="s">
-        <v>130</v>
-      </c>
-      <c r="C11" s="38" t="s">
-        <v>131</v>
-      </c>
-      <c r="D11" s="48" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="B12" s="45" t="s">
-        <v>133</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>131</v>
-      </c>
-      <c r="D12" s="48" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="37" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="46" t="s">
-        <v>185</v>
-      </c>
-      <c r="B13" s="47" t="s">
-        <v>186</v>
-      </c>
-      <c r="C13" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="D13" s="48" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="37" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="46" t="s">
-        <v>183</v>
-      </c>
-      <c r="B14" s="47" t="s">
-        <v>184</v>
-      </c>
-      <c r="C14" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="D14" s="48" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="37" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="46" t="s">
+      <c r="B23" s="43" t="s">
+        <v>169</v>
+      </c>
+      <c r="C23" s="36" t="s">
         <v>171</v>
       </c>
-      <c r="B15" s="47" t="s">
+      <c r="D23" s="47" t="s">
         <v>172</v>
       </c>
-      <c r="C15" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="D15" s="48" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="37" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="46" t="s">
+    </row>
+    <row r="24" spans="1:4" ht="28.9" x14ac:dyDescent="0.3">
+      <c r="A24" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="B24" s="48" t="s">
+        <v>181</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="D24" s="49" t="s">
         <v>154</v>
-      </c>
-      <c r="B16" s="47" t="s">
-        <v>156</v>
-      </c>
-      <c r="C16" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="D16" s="48" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
-        <v>155</v>
-      </c>
-      <c r="B17" s="47" t="s">
-        <v>157</v>
-      </c>
-      <c r="C17" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="D17" s="48" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="44" t="s">
-        <v>163</v>
-      </c>
-      <c r="B18" s="36" t="s">
-        <v>164</v>
-      </c>
-      <c r="C18" s="38" t="s">
-        <v>165</v>
-      </c>
-      <c r="D18" s="49" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="44" t="s">
-        <v>167</v>
-      </c>
-      <c r="B19" s="36" t="s">
-        <v>168</v>
-      </c>
-      <c r="C19" s="38">
-        <v>300</v>
-      </c>
-      <c r="D19" s="36" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="44" t="s">
-        <v>173</v>
-      </c>
-      <c r="B20" s="36" t="s">
-        <v>158</v>
-      </c>
-      <c r="C20" s="38" t="s">
-        <v>159</v>
-      </c>
-      <c r="D20" s="49" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="44" t="s">
-        <v>160</v>
-      </c>
-      <c r="B21" s="36" t="s">
-        <v>161</v>
-      </c>
-      <c r="C21" s="38" t="s">
-        <v>231</v>
-      </c>
-      <c r="D21" s="49" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="44" t="s">
-        <v>174</v>
-      </c>
-      <c r="B22" s="45" t="s">
-        <v>187</v>
-      </c>
-      <c r="C22" s="38" t="s">
-        <v>232</v>
-      </c>
-      <c r="D22" s="49" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="44" t="s">
-        <v>178</v>
-      </c>
-      <c r="B23" s="45" t="s">
-        <v>177</v>
-      </c>
-      <c r="C23" s="38" t="s">
-        <v>179</v>
-      </c>
-      <c r="D23" s="49" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="B24" s="50" t="s">
-        <v>189</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="D24" s="51" t="s">
-        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2340,200 +2441,203 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="73" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="51.109375" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="18"/>
+    <col min="4" max="4" width="73" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="9.140625" style="18"/>
+    <col min="9" max="9" width="51.140625" style="18" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:9" s="120" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="116" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="117" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="117" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="118" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="119" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="119" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="109" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="110" t="s">
+    <row r="2" spans="1:9" s="128" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="121" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="122" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="111" t="s">
+      <c r="C2" s="122" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="111" t="s">
+      <c r="D2" s="123" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="112">
+      <c r="E2" s="124">
         <v>1</v>
       </c>
-      <c r="F2" s="113">
+      <c r="F2" s="125">
         <v>10</v>
       </c>
-      <c r="G2" s="114"/>
-      <c r="H2" s="115"/>
-      <c r="I2" s="116" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="124" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="117" t="s">
-        <v>195</v>
-      </c>
-      <c r="B3" s="118" t="s">
+      <c r="G2" s="126"/>
+      <c r="H2" s="127"/>
+      <c r="I2" s="160" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="136" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="129" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3" s="130" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="118" t="s">
+      <c r="C3" s="130" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="118" t="s">
-        <v>223</v>
-      </c>
-      <c r="E3" s="119">
+      <c r="D3" s="131" t="s">
+        <v>214</v>
+      </c>
+      <c r="E3" s="132">
         <v>1458</v>
       </c>
-      <c r="F3" s="120">
+      <c r="F3" s="133">
         <v>873</v>
       </c>
-      <c r="G3" s="121"/>
-      <c r="H3" s="122"/>
-      <c r="I3" s="123" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="124" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="125" t="s">
-        <v>195</v>
-      </c>
-      <c r="B4" s="126" t="s">
+      <c r="G3" s="134"/>
+      <c r="H3" s="135"/>
+      <c r="I3" s="161" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="136" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="137" t="s">
+        <v>187</v>
+      </c>
+      <c r="B4" s="138" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="126" t="s">
+      <c r="C4" s="138" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="126" t="s">
+      <c r="D4" s="139" t="s">
         <v>85</v>
       </c>
-      <c r="E4" s="127">
+      <c r="E4" s="140">
         <v>10</v>
       </c>
-      <c r="F4" s="128">
+      <c r="F4" s="141">
         <v>0</v>
       </c>
-      <c r="G4" s="129"/>
-      <c r="H4" s="130">
+      <c r="G4" s="142"/>
+      <c r="H4" s="143">
         <v>-5</v>
       </c>
-      <c r="I4" s="131" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="124" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="132" t="s">
-        <v>195</v>
-      </c>
-      <c r="B5" s="133" t="s">
+      <c r="I4" s="162" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="136" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="144" t="s">
+        <v>187</v>
+      </c>
+      <c r="B5" s="145" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="133" t="s">
+      <c r="C5" s="145" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="133" t="s">
-        <v>192</v>
-      </c>
-      <c r="E5" s="134">
+      <c r="D5" s="146" t="s">
+        <v>184</v>
+      </c>
+      <c r="E5" s="147">
         <v>0.1</v>
       </c>
-      <c r="F5" s="135">
+      <c r="F5" s="148">
         <v>0</v>
       </c>
-      <c r="G5" s="136"/>
-      <c r="H5" s="137"/>
-      <c r="I5" s="138" t="s">
+      <c r="G5" s="149"/>
+      <c r="H5" s="150"/>
+      <c r="I5" s="163" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="108" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="139" t="s">
+    <row r="6" spans="1:9" s="155" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="151" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="140" t="s">
+      <c r="B6" s="152" t="s">
         <v>102</v>
       </c>
-      <c r="C6" s="140" t="s">
+      <c r="C6" s="152" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="140" t="s">
+      <c r="D6" s="153" t="s">
         <v>101</v>
       </c>
-      <c r="E6" s="139">
+      <c r="E6" s="151">
         <v>0.2</v>
       </c>
-      <c r="F6" s="140">
+      <c r="F6" s="152">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="G6" s="140">
+      <c r="G6" s="152">
         <v>0.09</v>
       </c>
-      <c r="H6" s="141"/>
-      <c r="I6" s="142" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="108" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="143" t="s">
+      <c r="H6" s="154"/>
+      <c r="I6" s="164" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="155" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="156" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="144" t="s">
-        <v>193</v>
-      </c>
-      <c r="C7" s="144" t="s">
+      <c r="B7" s="157" t="s">
+        <v>185</v>
+      </c>
+      <c r="C7" s="157" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="144" t="s">
-        <v>194</v>
-      </c>
-      <c r="E7" s="143">
+      <c r="D7" s="158" t="s">
+        <v>186</v>
+      </c>
+      <c r="E7" s="156">
         <v>0</v>
       </c>
-      <c r="F7" s="144">
+      <c r="F7" s="157">
         <v>0</v>
       </c>
-      <c r="G7" s="144">
+      <c r="G7" s="157">
         <v>0</v>
       </c>
-      <c r="H7" s="145"/>
-      <c r="I7" s="146" t="s">
-        <v>237</v>
+      <c r="H7" s="159"/>
+      <c r="I7" s="165" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -2550,265 +2654,265 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="93.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="93.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="31">
+      <c r="E1" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="34">
+      <c r="E2" s="32">
         <v>51.7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="E3" s="32">
+      <c r="E3" s="30">
         <v>0.2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="E4" s="32">
+      <c r="E4" s="30">
         <v>0.3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="E5" s="32">
+      <c r="E5" s="30">
         <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="30">
         <v>0.65</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="E10" s="150">
+      <c r="E10" s="106">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="E11" s="150">
+      <c r="E11" s="106">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="E12" s="150">
+      <c r="E12" s="106">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="52">
+      <c r="E13" s="50">
         <v>10000</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="E14" s="35">
+      <c r="E14" s="33">
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="124" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="132" t="s">
+    <row r="15" spans="1:5" s="102" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="103" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="133" t="s">
+      <c r="B15" s="104" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="133" t="s">
+      <c r="C15" s="104" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="133" t="s">
+      <c r="D15" s="104" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="157">
+      <c r="E15" s="113">
         <v>0.1</v>
       </c>
     </row>
@@ -2822,20 +2926,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="6"/>
-    <col min="4" max="4" width="71.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="6"/>
-    <col min="6" max="6" width="52.6640625" style="7" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="6"/>
+    <col min="1" max="1" width="12.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="6"/>
+    <col min="4" max="4" width="71.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="6"/>
+    <col min="6" max="6" width="52.7109375" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>69</v>
       </c>
@@ -2855,360 +2961,360 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="71" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+    <row r="2" spans="1:6" s="67" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="63" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="64" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="68" t="s">
+      <c r="C2" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="68" t="s">
+      <c r="D2" s="64" t="s">
         <v>109</v>
       </c>
-      <c r="E2" s="68">
+      <c r="E2" s="64">
         <v>0</v>
       </c>
-      <c r="F2" s="70"/>
-    </row>
-    <row r="3" spans="1:6" s="71" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="78" t="s">
+      <c r="F2" s="66"/>
+    </row>
+    <row r="3" spans="1:6" s="67" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="75" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="79" t="s">
+      <c r="C3" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="79" t="s">
+      <c r="D3" s="75" t="s">
         <v>112</v>
       </c>
-      <c r="E3" s="79">
+      <c r="E3" s="75">
         <v>2.74</v>
       </c>
-      <c r="F3" s="81"/>
-    </row>
-    <row r="4" spans="1:6" s="71" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="67" t="s">
+      <c r="F3" s="77"/>
+    </row>
+    <row r="4" spans="1:6" s="67" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="68" t="s">
-        <v>188</v>
-      </c>
-      <c r="C4" s="68" t="s">
+      <c r="B4" s="64" t="s">
+        <v>180</v>
+      </c>
+      <c r="C4" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="68" t="s">
+      <c r="D4" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="69">
+      <c r="E4" s="65">
         <v>0.02</v>
       </c>
-      <c r="F4" s="70"/>
-    </row>
-    <row r="5" spans="1:6" s="155" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="151" t="s">
+      <c r="F4" s="66"/>
+    </row>
+    <row r="5" spans="1:6" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="107" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="152" t="s">
+      <c r="B5" s="108" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="152" t="s">
+      <c r="C5" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="152" t="s">
+      <c r="D5" s="108" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="153">
+      <c r="E5" s="109">
         <v>1</v>
       </c>
-      <c r="F5" s="154" t="s">
+      <c r="F5" s="110" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="67" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="68" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="69" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="69" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="72">
+        <v>290</v>
+      </c>
+      <c r="F6" s="71"/>
+    </row>
+    <row r="7" spans="1:6" s="67" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="68" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="69" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="69" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="69" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="70">
+        <v>0.7</v>
+      </c>
+      <c r="F7" s="71"/>
+    </row>
+    <row r="8" spans="1:6" s="67" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="68" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="69" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="69" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="72">
+        <v>65</v>
+      </c>
+      <c r="F8" s="71"/>
+    </row>
+    <row r="9" spans="1:6" s="67" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="68" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="69" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="69" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="69" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="70">
+        <v>0.4</v>
+      </c>
+      <c r="F9" s="71"/>
+    </row>
+    <row r="10" spans="1:6" s="67" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="68" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="69" t="s">
+        <v>182</v>
+      </c>
+      <c r="C10" s="69" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="73">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="71"/>
+    </row>
+    <row r="11" spans="1:6" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="107" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="108" t="s">
+        <v>183</v>
+      </c>
+      <c r="C11" s="108" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="108" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="115">
+        <v>0.43</v>
+      </c>
+      <c r="F11" s="110" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="71" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="72" t="s">
+    <row r="12" spans="1:6" s="67" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="74" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="73" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="73" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="73" t="s">
-        <v>67</v>
-      </c>
-      <c r="E6" s="76">
-        <v>290</v>
-      </c>
-      <c r="F6" s="75"/>
-    </row>
-    <row r="7" spans="1:6" s="71" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="72" t="s">
-        <v>70</v>
-      </c>
-      <c r="B7" s="73" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="73" t="s">
+      <c r="B12" s="75" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="75" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="75" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="76">
+        <v>1</v>
+      </c>
+      <c r="F12" s="77"/>
+    </row>
+    <row r="13" spans="1:6" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="86" t="s">
+        <v>187</v>
+      </c>
+      <c r="B13" s="87" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="87" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="87" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="88">
+        <v>95</v>
+      </c>
+      <c r="F13" s="89" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="90" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="91" t="s">
+        <v>187</v>
+      </c>
+      <c r="B14" s="92" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="92" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="92" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="93">
+        <v>1.1315280460000001E-4</v>
+      </c>
+      <c r="F14" s="166" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="90" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="94" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="95" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="95" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="95" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="96">
+        <v>0.02</v>
+      </c>
+      <c r="F15" s="114"/>
+    </row>
+    <row r="16" spans="1:6" s="90" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="94" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="95" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="73" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="74">
-        <v>0.7</v>
-      </c>
-      <c r="F7" s="75"/>
-    </row>
-    <row r="8" spans="1:6" s="71" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="72" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="73" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="73" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="73" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="76">
-        <v>65</v>
-      </c>
-      <c r="F8" s="75"/>
-    </row>
-    <row r="9" spans="1:6" s="71" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="72" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" s="73" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="73" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="73" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="74">
-        <v>0.4</v>
-      </c>
-      <c r="F9" s="75"/>
-    </row>
-    <row r="10" spans="1:6" s="71" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="72" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="73" t="s">
-        <v>190</v>
-      </c>
-      <c r="C10" s="73" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="73" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="77">
-        <v>0.5</v>
-      </c>
-      <c r="F10" s="75"/>
-    </row>
-    <row r="11" spans="1:6" s="155" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="151" t="s">
-        <v>70</v>
-      </c>
-      <c r="B11" s="152" t="s">
-        <v>191</v>
-      </c>
-      <c r="C11" s="152" t="s">
+      <c r="D16" s="95" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="97">
+        <v>1.6</v>
+      </c>
+      <c r="F16" s="167" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="80" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="78" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="79" t="s">
+        <v>210</v>
+      </c>
+      <c r="C17" s="79" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="79" t="s">
+        <v>211</v>
+      </c>
+      <c r="E17" s="82">
+        <v>1500</v>
+      </c>
+      <c r="F17" s="81"/>
+    </row>
+    <row r="18" spans="1:6" s="80" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="83" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="84" t="s">
+        <v>209</v>
+      </c>
+      <c r="C18" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="152" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="159">
-        <v>0.43</v>
-      </c>
-      <c r="F11" s="154" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="71" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="78" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="79" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="79" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="79" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="80">
-        <v>1</v>
-      </c>
-      <c r="F12" s="81"/>
-    </row>
-    <row r="13" spans="1:6" s="94" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="90" t="s">
-        <v>195</v>
-      </c>
-      <c r="B13" s="91" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="91" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="91" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" s="92">
+      <c r="D18" s="84" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="105">
+        <v>2</v>
+      </c>
+      <c r="F18" s="85"/>
+    </row>
+    <row r="19" spans="1:6" s="80" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="98" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="99" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="99" t="s">
         <v>95</v>
       </c>
-      <c r="F13" s="93" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="94" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="95" t="s">
-        <v>195</v>
-      </c>
-      <c r="B14" s="96" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="96" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="96" t="s">
-        <v>106</v>
-      </c>
-      <c r="E14" s="97">
-        <v>1.1315280460000001E-4</v>
-      </c>
-      <c r="F14" s="98" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="94" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="99" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="100" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="100" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="100" t="s">
-        <v>65</v>
-      </c>
-      <c r="E15" s="101">
-        <v>0.02</v>
-      </c>
-      <c r="F15" s="158"/>
-    </row>
-    <row r="16" spans="1:6" s="94" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="99" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" s="100" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="100" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="100" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="102">
-        <v>1.6</v>
-      </c>
-      <c r="F16" s="148" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="84" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="82" t="s">
+      <c r="D19" s="99" t="s">
+        <v>98</v>
+      </c>
+      <c r="E19" s="99">
+        <v>60</v>
+      </c>
+      <c r="F19" s="168" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="80" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="100" t="s">
         <v>73</v>
       </c>
-      <c r="B17" s="83" t="s">
-        <v>219</v>
-      </c>
-      <c r="C17" s="83" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="83" t="s">
-        <v>220</v>
-      </c>
-      <c r="E17" s="86">
-        <v>1500</v>
-      </c>
-      <c r="F17" s="85"/>
-    </row>
-    <row r="18" spans="1:6" s="84" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="87" t="s">
-        <v>73</v>
-      </c>
-      <c r="B18" s="88" t="s">
-        <v>218</v>
-      </c>
-      <c r="C18" s="88" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="88" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="147">
-        <v>2</v>
-      </c>
-      <c r="F18" s="89"/>
-    </row>
-    <row r="19" spans="1:6" s="84" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="103" t="s">
-        <v>73</v>
-      </c>
-      <c r="B19" s="104" t="s">
-        <v>96</v>
-      </c>
-      <c r="C19" s="104" t="s">
+      <c r="B20" s="101" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" s="101" t="s">
         <v>95</v>
       </c>
-      <c r="D19" s="104" t="s">
-        <v>98</v>
-      </c>
-      <c r="E19" s="104">
-        <v>60</v>
-      </c>
-      <c r="F19" s="105" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="84" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="106" t="s">
-        <v>73</v>
-      </c>
-      <c r="B20" s="107" t="s">
-        <v>97</v>
-      </c>
-      <c r="C20" s="107" t="s">
-        <v>95</v>
-      </c>
-      <c r="D20" s="107" t="s">
+      <c r="D20" s="101" t="s">
         <v>99</v>
       </c>
-      <c r="E20" s="107">
+      <c r="E20" s="101">
         <v>304</v>
       </c>
-      <c r="F20" s="149" t="s">
-        <v>145</v>
+      <c r="F20" s="169" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -3219,51 +3325,53 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" style="3" customWidth="1"/>
     <col min="2" max="2" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="78.44140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="78.42578125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="3" customWidth="1"/>
     <col min="8" max="8" width="12" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="3"/>
+    <col min="9" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>33</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="156">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="112">
         <v>7.4999999999999993E-5</v>
       </c>
       <c r="B6" s="5">
@@ -3274,17 +3382,17 @@
         <v>4.0175999999999989E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>33</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>35</v>
@@ -3296,7 +3404,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>0.01</v>
       </c>
@@ -3317,285 +3425,236 @@
     </row>
     <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="62" t="s">
-        <v>196</v>
-      </c>
-      <c r="B14" s="63" t="s">
-        <v>197</v>
-      </c>
-      <c r="C14" s="62" t="s">
-        <v>198</v>
-      </c>
-      <c r="D14" s="63" t="s">
-        <v>199</v>
-      </c>
-      <c r="E14" s="64" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="58" t="s">
+        <v>188</v>
+      </c>
+      <c r="B14" s="59" t="s">
+        <v>189</v>
+      </c>
+      <c r="C14" s="58" t="s">
+        <v>190</v>
+      </c>
+      <c r="D14" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="E14" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="62" t="s">
+      <c r="F14" s="58" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="55" t="s">
-        <v>215</v>
-      </c>
-      <c r="B15" s="56">
+      <c r="A15" s="51" t="s">
+        <v>206</v>
+      </c>
+      <c r="B15" s="52">
         <v>1000</v>
       </c>
-      <c r="C15" s="57">
+      <c r="C15" s="53">
         <v>100</v>
       </c>
-      <c r="D15" s="56">
+      <c r="D15" s="52">
         <v>2650</v>
       </c>
-      <c r="E15" s="58" t="s">
+      <c r="E15" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="F15" s="66" t="s">
-        <v>216</v>
+      <c r="F15" s="62" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="57" t="s">
+      <c r="A16" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="56">
+      <c r="B16" s="52">
         <v>10</v>
       </c>
-      <c r="C16" s="57">
+      <c r="C16" s="53">
         <v>5</v>
       </c>
-      <c r="D16" s="56">
+      <c r="D16" s="52">
         <v>30</v>
       </c>
-      <c r="E16" s="58" t="s">
+      <c r="E16" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="66" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="59" t="s">
+      <c r="F16" s="62" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="60">
+      <c r="B17" s="56">
         <f>B15*B16/100</f>
         <v>100</v>
       </c>
-      <c r="C17" s="59">
+      <c r="C17" s="55">
         <f>C15*C16/100</f>
         <v>5</v>
       </c>
-      <c r="D17" s="60">
+      <c r="D17" s="56">
         <f>D15*D16/100</f>
         <v>795</v>
       </c>
-      <c r="E17" s="61" t="s">
+      <c r="E17" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="F17" s="65"/>
-    </row>
-    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="F17" s="61"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="B21" s="53">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="177" t="s">
+        <v>192</v>
+      </c>
+      <c r="B20" s="178" t="s">
+        <v>193</v>
+      </c>
+      <c r="C20" s="179" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="170" t="s">
+        <v>194</v>
+      </c>
+      <c r="B21" s="171">
         <v>0.1</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="172">
         <f>B21*1000</f>
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="B22" s="54">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="170" t="s">
+        <v>195</v>
+      </c>
+      <c r="B22" s="173">
         <v>1</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="172">
         <f t="shared" ref="C22:C31" si="0">B22*1000</f>
         <v>1000</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="B23" s="53">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="170" t="s">
+        <v>196</v>
+      </c>
+      <c r="B23" s="171">
         <v>1.2</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="172">
         <f t="shared" si="0"/>
         <v>1200</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="B24" s="53">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="170" t="s">
+        <v>197</v>
+      </c>
+      <c r="B24" s="171">
         <v>1.4</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="172">
         <f t="shared" si="0"/>
         <v>1400</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="B25" s="53">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="170" t="s">
+        <v>197</v>
+      </c>
+      <c r="B25" s="171">
         <v>1.35</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="172">
         <f t="shared" si="0"/>
         <v>1350</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="B26" s="53">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="170" t="s">
+        <v>198</v>
+      </c>
+      <c r="B26" s="171">
         <v>1.35</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="172">
         <f t="shared" si="0"/>
         <v>1350</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="B27" s="53">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="170" t="s">
+        <v>199</v>
+      </c>
+      <c r="B27" s="171">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="172">
         <f t="shared" si="0"/>
         <v>1100</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="B28" s="53">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="170" t="s">
+        <v>200</v>
+      </c>
+      <c r="B28" s="171">
         <v>1.8</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="172">
         <f t="shared" si="0"/>
         <v>1800</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="B29" s="53">
+      <c r="A29" s="170" t="s">
+        <v>201</v>
+      </c>
+      <c r="B29" s="171">
         <v>1.7</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="172">
         <f t="shared" si="0"/>
         <v>1700</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="B30" s="53">
+      <c r="A30" s="170" t="s">
+        <v>202</v>
+      </c>
+      <c r="B30" s="171">
         <v>1.65</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="172">
         <f t="shared" si="0"/>
         <v>1650</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="B31" s="53">
+      <c r="A31" s="174" t="s">
+        <v>203</v>
+      </c>
+      <c r="B31" s="175">
         <v>2.65</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="176">
         <f t="shared" si="0"/>
         <v>2650</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A34" s="18" t="s">
-        <v>142</v>
-      </c>
-      <c r="F34" s="38" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A35" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="F35" s="38" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A36" s="18" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A39" s="19" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A40" s="19" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A41" s="19" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>